<commit_message>
fix 2s point bug
</commit_message>
<xml_diff>
--- a/src/main/resources/SH600511.xlsx
+++ b/src/main/resources/SH600511.xlsx
@@ -2424,11 +2424,21 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>20210309</t>
+          <t>20210325</t>
         </is>
       </c>
       <c r="B237" t="n">
-        <v>3338.0</v>
+        <v>3291.0</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>20210331</t>
+        </is>
+      </c>
+      <c r="B238" t="n">
+        <v>3465.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>